<commit_message>
Fixed: Prioritised macOS compatibility
</commit_message>
<xml_diff>
--- a/21S2AccrSurvey_EEXXXX-Results (ready).xlsx
+++ b/21S2AccrSurvey_EEXXXX-Results (ready).xlsx
@@ -4848,7 +4848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N161"/>
+  <dimension ref="A1:N179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
@@ -6619,6 +6619,132 @@
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">test </t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">comments </t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">comments </t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">comments </t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">testing </t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>testing 2:07pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">testing </t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
         <is>
           <t xml:space="preserve">test </t>
         </is>
@@ -6650,7 +6776,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N151"/>
+  <dimension ref="A1:N160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="99" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -8316,6 +8442,69 @@
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">testing </t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cljx laptop </t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">testing </t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>test 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">testing </t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
         <is>
           <t>.</t>
         </is>

</xml_diff>